<commit_message>
Update to fit the changed sugangsnu data schema
</commit_message>
<xml_diff>
--- a/test/batch/coursebook/sugangsnu/SugangSnuTestExcel.xlsx
+++ b/test/batch/coursebook/sugangsnu/SugangSnuTestExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_a1b\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hankchoi/git-public/snutt/test/batch/coursebook/sugangsnu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9656017-911C-424D-BDDA-C0AF91E4D69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224420EB-D18A-6345-89D4-671E1E1A23ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="74">
   <si>
     <t>강좌검색</t>
   </si>
@@ -247,13 +245,19 @@
   </si>
   <si>
     <t>1. 그린리더십 교과목 2과목 선이수 학생대상-2018학년도 1학기 수강중인 과목도 선이수 과목에 포함됨/2. 지원서와 자기 소개서 제출 http://aiees.snu.ac.kr/greenleadership/home /문의: 880-2665</t>
+  </si>
+  <si>
+    <t>재학생장바구니신청</t>
+  </si>
+  <si>
+    <t>신입생장바구니신청</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -267,6 +271,12 @@
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="나눔고딕OTF"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="3">
@@ -321,10 +331,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -343,7 +353,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -639,83 +649,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="9" width="19.5703125" customWidth="1"/>
-    <col min="10" max="12" width="5.85546875" customWidth="1"/>
-    <col min="13" max="13" width="19.5703125" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" customWidth="1"/>
-    <col min="16" max="19" width="7.85546875" customWidth="1"/>
-    <col min="20" max="20" width="15.5703125" customWidth="1"/>
-    <col min="21" max="22" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="9" width="19.5" customWidth="1"/>
+    <col min="10" max="12" width="5.83203125" customWidth="1"/>
+    <col min="13" max="13" width="19.5" customWidth="1"/>
+    <col min="14" max="14" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="19.5" customWidth="1"/>
+    <col min="16" max="21" width="7.83203125" customWidth="1"/>
+    <col min="22" max="22" width="15.5" customWidth="1"/>
+    <col min="23" max="24" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="20.25">
+    <row r="1" spans="1:24" ht="20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
     </row>
-    <row r="2" spans="1:22" ht="15.75">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:24" ht="16">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:24">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -768,22 +782,28 @@
         <v>18</v>
       </c>
       <c r="R3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:24">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -836,22 +856,28 @@
         <v>0</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:24">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -904,22 +930,28 @@
         <v>1</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="U5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:24">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -972,22 +1004,28 @@
         <v>2</v>
       </c>
       <c r="R6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:24">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1040,22 +1078,28 @@
         <v>3</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:24">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -1108,22 +1152,28 @@
         <v>4</v>
       </c>
       <c r="R8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="W8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="X8" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:24">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1176,22 +1226,28 @@
         <v>5</v>
       </c>
       <c r="R9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="W9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="X9" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:24">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1244,22 +1300,28 @@
         <v>6</v>
       </c>
       <c r="R10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:24">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -1312,22 +1374,28 @@
         <v>7</v>
       </c>
       <c r="R11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="U11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="V11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="W11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="X11" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:24">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1380,26 +1448,33 @@
         <v>8</v>
       </c>
       <c r="R12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="U12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="W12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="X12" s="1" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:V1"/>
-    <mergeCell ref="A2:V2"/>
+    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="A2:X2"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>